<commit_message>
Updates student marks spreadsheet
Refreshes the student marks data. This ensures the accuracy.
</commit_message>
<xml_diff>
--- a/student_marks.xlsx
+++ b/student_marks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Documents\GitHub\CHATBOT-DEMO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1D0E26-D713-44BB-B2E9-20DF367BD91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E098B43-40E9-4595-8C9B-30390A2A984E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{100CBAB8-14D5-42E9-A86D-1D0F29D63044}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>StudentID</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Mary</t>
+  </si>
+  <si>
+    <t>Sidhaarth</t>
+  </si>
+  <si>
+    <t>Social Science</t>
   </si>
 </sst>
 </file>
@@ -423,13 +429,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EB2088-8E00-4D61-8BB5-E61F41E5FF5A}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -481,10 +490,52 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>102</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D5" s="2">
         <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>103</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>101</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Converted to a easy-to-read format.
</commit_message>
<xml_diff>
--- a/student_marks.xlsx
+++ b/student_marks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Documents\GitHub\CHATBOT-DEMO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E098B43-40E9-4595-8C9B-30390A2A984E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D7C172-6BFE-476A-A5DD-03771C1E896F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{100CBAB8-14D5-42E9-A86D-1D0F29D63044}"/>
   </bookViews>
@@ -34,20 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
-  <si>
-    <t>StudentID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Marks</t>
-  </si>
-  <si>
     <t>John</t>
   </si>
   <si>
@@ -60,10 +51,22 @@
     <t>Mary</t>
   </si>
   <si>
-    <t>Sidhaarth</t>
-  </si>
-  <si>
-    <t>Social Science</t>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>David</t>
   </si>
 </sst>
 </file>
@@ -429,113 +432,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EB2088-8E00-4D61-8BB5-E61F41E5FF5A}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>101</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2">
+        <v>85</v>
+      </c>
+      <c r="C3" s="2">
+        <v>78</v>
+      </c>
+      <c r="D3" s="2">
+        <v>92</v>
+      </c>
+      <c r="E3" s="2">
+        <v>65</v>
+      </c>
+      <c r="F3" s="2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
-        <v>101</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>102</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
+      <c r="B4" s="2">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2">
+        <v>42</v>
       </c>
       <c r="D4" s="2">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>102</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>38</v>
+      </c>
+      <c r="E4" s="2">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <v>100</v>
+      </c>
+      <c r="C5" s="2">
+        <v>95</v>
       </c>
       <c r="D5" s="2">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>103</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="2">
+        <v>98</v>
+      </c>
+      <c r="F5" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B6" s="2">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2">
+        <v>33</v>
+      </c>
       <c r="D6" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>101</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
+      </c>
+      <c r="E6" s="2">
+        <v>50</v>
+      </c>
+      <c r="F6" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2">
+        <v>55</v>
       </c>
       <c r="D7" s="2">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="E7" s="2">
+        <v>65</v>
+      </c>
+      <c r="F7" s="2">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the data to easy-to-read format.
</commit_message>
<xml_diff>
--- a/student_marks.xlsx
+++ b/student_marks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Documents\GitHub\CHATBOT-DEMO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D7C172-6BFE-476A-A5DD-03771C1E896F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7F9627-978E-4414-BFBB-734F3602D6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{100CBAB8-14D5-42E9-A86D-1D0F29D63044}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{100CBAB8-14D5-42E9-A86D-1D0F29D63044}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added logistic regression prediction option & added a column to excel data.
</commit_message>
<xml_diff>
--- a/student_marks.xlsx
+++ b/student_marks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Documents\GitHub\CHATBOT-DEMO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7F9627-978E-4414-BFBB-734F3602D6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CF5DD7-DDFE-49C5-AA82-95EF5F4FDBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{100CBAB8-14D5-42E9-A86D-1D0F29D63044}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="12310" windowHeight="6870" xr2:uid="{100CBAB8-14D5-42E9-A86D-1D0F29D63044}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EB2088-8E00-4D61-8BB5-E61F41E5FF5A}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -445,128 +445,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>85</v>
+      </c>
+      <c r="C2" s="2">
+        <v>78</v>
+      </c>
+      <c r="D2" s="2">
+        <v>92</v>
+      </c>
+      <c r="E2" s="2">
+        <v>65</v>
+      </c>
+      <c r="F2" s="2">
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="C3" s="2">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="E3" s="2">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="F3" s="2">
-        <v>88</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="C4" s="2">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D4" s="2">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="E4" s="2">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="F4" s="2">
-        <v>45</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
-        <v>100</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="E5" s="2">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="F5" s="2">
-        <v>99</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="D6" s="2">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E6" s="2">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="F6" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2">
-        <v>60</v>
-      </c>
-      <c r="C7" s="2">
-        <v>55</v>
-      </c>
-      <c r="D7" s="2">
-        <v>70</v>
-      </c>
-      <c r="E7" s="2">
-        <v>65</v>
-      </c>
-      <c r="F7" s="2">
         <v>80</v>
       </c>
     </row>

</xml_diff>